<commit_message>
I don't know quite what this is
</commit_message>
<xml_diff>
--- a/test262/Tests.xlsx
+++ b/test262/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="3640" windowWidth="35620" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="2700" windowWidth="35620" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="141">
   <si>
     <t>Passing</t>
   </si>
@@ -336,9 +336,6 @@
   </si>
   <si>
     <t>S9.3_A5_T2.js: div 0</t>
-  </si>
-  <si>
-    <t>11.13.2-47-s.js: mod with NaN</t>
   </si>
   <si>
     <t>S11.13.2_A3.1_T3.js: ???</t>
@@ -1043,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I60" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="L74" sqref="L74"/>
+    <sheetView tabSelected="1" topLeftCell="J57" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2596,16 +2593,13 @@
       <c r="C35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="36" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>93</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="3:25" x14ac:dyDescent="0.2">
@@ -2613,7 +2607,7 @@
         <v>94</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="3:25" x14ac:dyDescent="0.2">
@@ -2621,7 +2615,7 @@
         <v>95</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="3:25" x14ac:dyDescent="0.2">
@@ -2629,7 +2623,7 @@
         <v>96</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.2">
@@ -2637,7 +2631,7 @@
         <v>97</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="3:25" x14ac:dyDescent="0.2">
@@ -2645,7 +2639,7 @@
         <v>98</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="3:25" x14ac:dyDescent="0.2">
@@ -2653,7 +2647,7 @@
         <v>99</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="3:25" x14ac:dyDescent="0.2">
@@ -2661,7 +2655,7 @@
         <v>100</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="3:25" x14ac:dyDescent="0.2">
@@ -2669,7 +2663,7 @@
         <v>101</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.2">
@@ -2677,147 +2671,147 @@
         <v>102</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L47" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L48" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L49" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L50" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L51" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L52" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L53" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L54" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L55" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L56" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L57" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L58" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L59" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L60" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L61" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L62" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L63" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L65" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L66" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L67" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L68" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L69" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L70" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L71" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L72" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L73" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>